<commit_message>
something shop blog admin
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C108D731-9AA3-4E56-884A-A6B4658A60B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AAB504-280C-463F-ADFE-EC23F69BA8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Todo</t>
   </si>
@@ -120,6 +121,27 @@
   </si>
   <si>
     <t>لاگین از گوگل</t>
+  </si>
+  <si>
+    <t>confirm email and phone number</t>
+  </si>
+  <si>
+    <t>ارسال اس ام اس</t>
+  </si>
+  <si>
+    <t>ارسال ایمیل</t>
+  </si>
+  <si>
+    <t>ثبت نام</t>
+  </si>
+  <si>
+    <t>تغییر رمز پروفایل</t>
+  </si>
+  <si>
+    <t>آدرس ها</t>
+  </si>
+  <si>
+    <t>سفارشات</t>
   </si>
 </sst>
 </file>
@@ -483,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,8 +545,8 @@
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -535,27 +557,27 @@
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
@@ -565,34 +587,49 @@
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -604,14 +641,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
product and user shopping cart
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AAB504-280C-463F-ADFE-EC23F69BA8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C252410-2998-4C19-AAE3-DA2F7C348523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Todo</t>
   </si>
@@ -142,6 +141,24 @@
   </si>
   <si>
     <t>سفارشات</t>
+  </si>
+  <si>
+    <t>زمانی که محصول به سبد خرید اضافه می شود. صفحه اتمام موجودی</t>
+  </si>
+  <si>
+    <t>اطلاعات فاکتور ا و سبد خرید در ادمین</t>
+  </si>
+  <si>
+    <t>کاربران و نقش ها در ادمین</t>
+  </si>
+  <si>
+    <t>نهایی کردن سفارش</t>
+  </si>
+  <si>
+    <t>حذف از سبد خرید</t>
+  </si>
+  <si>
+    <t>سئو در صفحه اصلی</t>
   </si>
 </sst>
 </file>
@@ -505,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +563,9 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -555,15 +575,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -574,7 +594,10 @@
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -583,77 +606,85 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
home base index and shop categories
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144C8C68-61B1-4EDA-8757-D48E7AB37016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D26FDDB-651B-424B-8FDF-E36C5BA236D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -606,7 +606,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,9 +643,6 @@
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
@@ -656,15 +653,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -674,27 +674,33 @@
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
@@ -704,6 +710,9 @@
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
@@ -772,10 +781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>63</v>
-      </c>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
@@ -788,18 +794,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>67</v>
-      </c>
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>68</v>
-      </c>
+    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
route for last site map
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3859B24-F46B-4E09-BBE4-08608ECA1A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB1542A-D079-424D-AB2A-66BD1AF7CEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Todo</t>
   </si>
@@ -258,6 +258,18 @@
   </si>
   <si>
     <t>تعداد یازدید ها</t>
+  </si>
+  <si>
+    <t>فوتر</t>
+  </si>
+  <si>
+    <t>تصویر داریان در سوشال مدیا</t>
+  </si>
+  <si>
+    <t>تگ ها درست نت</t>
+  </si>
+  <si>
+    <t>تصاویر پنل ادمین</t>
   </si>
 </sst>
 </file>
@@ -621,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,22 +676,16 @@
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
@@ -692,9 +698,6 @@
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
@@ -706,9 +709,6 @@
       <c r="D5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
@@ -717,9 +717,6 @@
       <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
@@ -800,86 +797,98 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="F26" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F27" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="F28" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="F29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="F30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="F31" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="F32" s="1" t="s">
         <v>51</v>
       </c>
@@ -952,6 +961,31 @@
     <row r="46" spans="6:6" ht="30" x14ac:dyDescent="0.25">
       <c r="F46" s="1" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F48" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F50" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
صفحات faq terms about contact
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB1542A-D079-424D-AB2A-66BD1AF7CEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3ED811-3A45-4F09-901D-741143840C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Todo</t>
   </si>
@@ -270,6 +270,18 @@
   </si>
   <si>
     <t>تصاویر پنل ادمین</t>
+  </si>
+  <si>
+    <t>home faq about comditions</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>ثبت لاگ بازدید بلاگ و لینک های ورودی</t>
+  </si>
+  <si>
+    <t>courses</t>
   </si>
 </sst>
 </file>
@@ -633,20 +645,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -666,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -680,7 +692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
@@ -691,7 +703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
@@ -702,7 +714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -713,7 +725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
@@ -721,18 +733,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
@@ -740,7 +749,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
@@ -748,7 +757,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
@@ -756,7 +765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
@@ -764,7 +773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
@@ -772,7 +781,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>70</v>
       </c>
@@ -780,7 +789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
@@ -788,204 +797,229 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F26" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F28" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F31" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F32" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F33" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F34" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F35" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F36" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F37" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F38" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F39" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F40" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F41" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="6:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F42" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="6:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="F43" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="6:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="F44" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F45" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F46" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F47" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F48" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F49" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F50" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F51" s="1" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F52" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F53" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F54" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="F55" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F56" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some bugs fixed (is published field did not worked) convert to webp added all images links removed and added reference to media id
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD545749-48F6-4564-B066-14C74F29639A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ED299E-03AB-41E6-A63E-C7B87ACFF657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>Todo</t>
   </si>
@@ -294,16 +294,36 @@
   </si>
   <si>
     <t>id of all images instead of link</t>
+  </si>
+  <si>
+    <t>لوگو های سایت کانفیگ</t>
+  </si>
+  <si>
+    <t>سابقه صفحات</t>
+  </si>
+  <si>
+    <t>کتاب خوان</t>
+  </si>
+  <si>
+    <t>افزودن استایل</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,10 +352,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -343,8 +364,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -659,18 +684,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -690,14 +715,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -707,7 +732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
@@ -721,10 +746,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -732,7 +760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
@@ -743,7 +771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
@@ -751,7 +779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
@@ -759,7 +787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>54</v>
       </c>
@@ -767,7 +795,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
@@ -775,7 +803,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>65</v>
       </c>
@@ -783,7 +811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
@@ -791,7 +819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
@@ -799,7 +827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>70</v>
       </c>
@@ -807,7 +835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
@@ -815,7 +843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>76</v>
       </c>
@@ -823,7 +851,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>78</v>
       </c>
@@ -831,7 +859,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>83</v>
       </c>
@@ -839,7 +867,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>80</v>
       </c>
@@ -847,7 +875,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>82</v>
       </c>
@@ -855,200 +883,212 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="F23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F26" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F27" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F28" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F31" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F32" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F33" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F34" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F35" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F36" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F37" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F38" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F39" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F40" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F41" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="6:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F42" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="6:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="F43" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="6:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="F44" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F45" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F46" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F47" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F48" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F49" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F50" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F51" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F52" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F53" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F54" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F55" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F56" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F57" s="1" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{ABF3B0EC-843F-4AF8-BFD5-62A5BDD80C4A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
price tag fixed for out of stock products products banner image fixed
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FB39C1-56A3-4DFA-B9E5-CD609EC39B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7527C5C1-4A89-4156-92F7-DDAE146CE687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
   <si>
     <t>Todo</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>مدت زمان لاگین ماندن</t>
+  </si>
+  <si>
+    <t>محصول ناموجود در لیست</t>
+  </si>
+  <si>
+    <t>محصول ناموجود در نمایش محصول</t>
+  </si>
+  <si>
+    <t>تخفیف های ویژه محصوا ناموجود</t>
   </si>
 </sst>
 </file>
@@ -675,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,6 +1105,26 @@
         <v>92</v>
       </c>
     </row>
+    <row r="64" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F65" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="F66" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="6:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F67" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
banner image in shop fixed
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7527C5C1-4A89-4156-92F7-DDAE146CE687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD89EBB-5637-4E36-B874-39EF0780C923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>Todo</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>تخفیف های ویژه محصوا ناموجود</t>
+  </si>
+  <si>
+    <t>آدر س صفحات برند ها</t>
+  </si>
+  <si>
+    <t>ثبت برند و محصول جدید توضیح نمی تواند خالی باشد</t>
   </si>
 </sst>
 </file>
@@ -687,7 +693,7 @@
   <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,6 +730,9 @@
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
@@ -895,7 +904,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
brand names added in url for shop products count fixed in brand pages
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD89EBB-5637-4E36-B874-39EF0780C923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23A601A-5CC3-4FD5-A19C-6B555EE2DBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,11 +730,11 @@
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="D2" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
main site logo fixed
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23A601A-5CC3-4FD5-A19C-6B555EE2DBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1B8BF4-775E-498A-8CB8-F3C71E455290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -690,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,9 +733,6 @@
       <c r="D2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1135,6 +1132,11 @@
     <row r="67" spans="6:6" ht="30" x14ac:dyDescent="0.25">
       <c r="F67" s="1" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F68" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
admin panel system change
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\BlogAndShopSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A40679E-8A31-4A9E-86FF-BD8BE90336FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1E0202-2D93-485E-B18F-B2FD886EF187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{29C67DDB-7497-47DA-A63C-07D42FAED0C7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>Todo</t>
   </si>
@@ -330,6 +330,21 @@
   </si>
   <si>
     <t>old tag pages</t>
+  </si>
+  <si>
+    <t>وسط چین بودن عکس های بلاگ</t>
+  </si>
+  <si>
+    <t>مطالب پیشنهادی وبلاگ بیش از 6 است</t>
+  </si>
+  <si>
+    <t>admin panel get global</t>
+  </si>
+  <si>
+    <t>یادآور ثبت محتوا</t>
+  </si>
+  <si>
+    <t>زمانبندی ارسال محتوا</t>
   </si>
 </sst>
 </file>
@@ -695,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D7E5F-9044-4FAA-AA3B-F7EA54359B5C}">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +777,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>31</v>
@@ -775,6 +790,9 @@
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>66</v>
       </c>
@@ -782,9 +800,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>84</v>
@@ -874,6 +895,9 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>43</v>
       </c>
@@ -903,11 +927,17 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>